<commit_message>
added top 10s  to overl P&L
</commit_message>
<xml_diff>
--- a/uploaded_files/Hanif+Rajput+Catering+Services_Profit+and+Loss-8.xlsx
+++ b/uploaded_files/Hanif+Rajput+Catering+Services_Profit+and+Loss-8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adnan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adnan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2FAD2B-BDDA-0D4E-9705-96E18DE764C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F605CB00-F355-6B45-90CE-32F0F5823FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,15 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Mar 2024</t>
-  </si>
-  <si>
-    <t>Mar 2023 (PP)</t>
+    <t>1 Jul, 2023 - 30 Mar, 2024</t>
+  </si>
+  <si>
+    <t>1 Jul, 2022 - 30 Mar, 2023 (PP)</t>
   </si>
   <si>
     <t>Income</t>
@@ -269,6 +269,9 @@
     <t xml:space="preserve">      100201 Office Rent</t>
   </si>
   <si>
+    <t xml:space="preserve">      100203 Token Tax</t>
+  </si>
+  <si>
     <t xml:space="preserve">      100204 Toll Tax</t>
   </si>
   <si>
@@ -281,6 +284,9 @@
     <t xml:space="preserve">      100301 Elecricity Charges</t>
   </si>
   <si>
+    <t xml:space="preserve">      100302 Gas Charges</t>
+  </si>
+  <si>
     <t xml:space="preserve">      100305 Water Charges</t>
   </si>
   <si>
@@ -290,6 +296,9 @@
     <t xml:space="preserve">   1004 Legal &amp; Professional Charges</t>
   </si>
   <si>
+    <t xml:space="preserve">      100401 Audit Fee</t>
+  </si>
+  <si>
     <t xml:space="preserve">      100402 Filing Fee</t>
   </si>
   <si>
@@ -299,6 +308,9 @@
     <t xml:space="preserve">      100404 Professional Services</t>
   </si>
   <si>
+    <t xml:space="preserve">      100405 Registration Fee</t>
+  </si>
+  <si>
     <t xml:space="preserve">      100406 Fee &amp; Subcription</t>
   </si>
   <si>
@@ -419,7 +431,7 @@
     <t>Net Earnings</t>
   </si>
   <si>
-    <t>Monday, Apr 01, 2024 06:48:05 PM GMT+5 - Accrual Basis</t>
+    <t>Saturday, Mar 30, 2024 02:11:39 PM GMT+5 - Accrual Basis</t>
   </si>
   <si>
     <t>Hanif Rajput Catering Services</t>
@@ -428,7 +440,7 @@
     <t>Profit and Loss</t>
   </si>
   <si>
-    <t>March 2024</t>
+    <t>1 July, 2023 - 30 March, 2024</t>
   </si>
 </sst>
 </file>
@@ -902,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C135"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -916,21 +928,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -942,7 +954,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="27" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -963,12 +975,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="5">
-        <f>33608003.2</f>
-        <v>33608003.200000003</v>
+        <f>200839444.89</f>
+        <v>200839444.88999999</v>
       </c>
       <c r="C8" s="5">
-        <f>49499252.55</f>
-        <v>49499252.549999997</v>
+        <f>182811116.9</f>
+        <v>182811116.90000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -983,12 +995,12 @@
         <v>6</v>
       </c>
       <c r="B10" s="5">
-        <f>200000</f>
-        <v>200000</v>
+        <f>12726000</f>
+        <v>12726000</v>
       </c>
       <c r="C10" s="5">
-        <f>3757000</f>
-        <v>3757000</v>
+        <f>25184739</f>
+        <v>25184739</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -997,11 +1009,11 @@
       </c>
       <c r="B11" s="6">
         <f>(B9)+(B10)</f>
-        <v>200000</v>
+        <v>12726000</v>
       </c>
       <c r="C11" s="6">
         <f>(C9)+(C10)</f>
-        <v>3757000</v>
+        <v>25184739</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1016,12 +1028,12 @@
         <v>9</v>
       </c>
       <c r="B13" s="5">
-        <f>7745123</f>
-        <v>7745123</v>
+        <f>81422675.5</f>
+        <v>81422675.5</v>
       </c>
       <c r="C13" s="5">
-        <f>16363873.91</f>
-        <v>16363873.91</v>
+        <f>88376502.44</f>
+        <v>88376502.439999998</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1029,12 +1041,12 @@
         <v>10</v>
       </c>
       <c r="B14" s="5">
-        <f>586939.3</f>
-        <v>586939.30000000005</v>
+        <f>5269320.3</f>
+        <v>5269320.3</v>
       </c>
       <c r="C14" s="5">
-        <f>516448</f>
-        <v>516448</v>
+        <f>5794517</f>
+        <v>5794517</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1043,11 +1055,11 @@
       </c>
       <c r="B15" s="6">
         <f>((B12)+(B13))+(B14)</f>
-        <v>8332062.2999999998</v>
+        <v>86691995.799999997</v>
       </c>
       <c r="C15" s="6">
         <f>((C12)+(C13))+(C14)</f>
-        <v>16880321.91</v>
+        <v>94171019.439999998</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1055,12 +1067,12 @@
         <v>12</v>
       </c>
       <c r="B16" s="5">
-        <f>535880</f>
-        <v>535880</v>
+        <f>7870780</f>
+        <v>7870780</v>
       </c>
       <c r="C16" s="5">
-        <f>1381550</f>
-        <v>1381550</v>
+        <f>7126955</f>
+        <v>7126955</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1068,22 +1080,25 @@
         <v>13</v>
       </c>
       <c r="B17" s="5">
-        <f>2412988</f>
-        <v>2412988</v>
+        <f>22302630</f>
+        <v>22302630</v>
       </c>
       <c r="C17" s="5">
-        <f>2535150</f>
-        <v>2535150</v>
+        <f>19585207.1</f>
+        <v>19585207.100000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="5">
+        <f>982750</f>
+        <v>982750</v>
+      </c>
       <c r="C18" s="5">
-        <f>147500</f>
-        <v>147500</v>
+        <f>1670120</f>
+        <v>1670120</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1091,12 +1106,12 @@
         <v>15</v>
       </c>
       <c r="B19" s="5">
-        <f>39800</f>
-        <v>39800</v>
+        <f>1363800</f>
+        <v>1363800</v>
       </c>
       <c r="C19" s="5">
-        <f>203200</f>
-        <v>203200</v>
+        <f>1216600</f>
+        <v>1216600</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,11 +1120,11 @@
       </c>
       <c r="B20" s="6">
         <f>((((((B8)+(B11))+(B15))+(B16))+(B17))+(B18))+(B19)</f>
-        <v>45128733.5</v>
+        <v>332777400.69</v>
       </c>
       <c r="C20" s="6">
         <f>((((((C8)+(C11))+(C15))+(C16))+(C17))+(C18))+(C19)</f>
-        <v>74403974.459999993</v>
+        <v>331765757.44000006</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1138,12 +1153,12 @@
         <v>20</v>
       </c>
       <c r="B24" s="5">
-        <f>1378206</f>
-        <v>1378206</v>
+        <f>23775608</f>
+        <v>23775608</v>
       </c>
       <c r="C24" s="5">
-        <f>4146089</f>
-        <v>4146089</v>
+        <f>24046624</f>
+        <v>24046624</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1151,12 +1166,12 @@
         <v>21</v>
       </c>
       <c r="B25" s="5">
-        <f>4222087</f>
-        <v>4222087</v>
+        <f>31584301</f>
+        <v>31584301</v>
       </c>
       <c r="C25" s="5">
-        <f>11171353</f>
-        <v>11171353</v>
+        <f>36158003.28</f>
+        <v>36158003.280000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1164,12 +1179,12 @@
         <v>22</v>
       </c>
       <c r="B26" s="5">
-        <f>1437649</f>
-        <v>1437649</v>
+        <f>5784255</f>
+        <v>5784255</v>
       </c>
       <c r="C26" s="5">
-        <f>1169406</f>
-        <v>1169406</v>
+        <f>4459168</f>
+        <v>4459168</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1177,12 +1192,12 @@
         <v>23</v>
       </c>
       <c r="B27" s="5">
-        <f>77000</f>
-        <v>77000</v>
+        <f>4083157</f>
+        <v>4083157</v>
       </c>
       <c r="C27" s="5">
-        <f>230800</f>
-        <v>230800</v>
+        <f>4295326</f>
+        <v>4295326</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1191,11 +1206,11 @@
       </c>
       <c r="B28" s="6">
         <f>((((B23)+(B24))+(B25))+(B26))+(B27)</f>
-        <v>7114942</v>
+        <v>65227321</v>
       </c>
       <c r="C28" s="6">
         <f>((((C23)+(C24))+(C25))+(C26))+(C27)</f>
-        <v>16717648</v>
+        <v>68959121.280000001</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1210,12 +1225,12 @@
         <v>26</v>
       </c>
       <c r="B30" s="5">
-        <f>1112324</f>
-        <v>1112324</v>
+        <f>7376256</f>
+        <v>7376256</v>
       </c>
       <c r="C30" s="5">
-        <f>842678</f>
-        <v>842678</v>
+        <f>8693172.76</f>
+        <v>8693172.7599999998</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1223,12 +1238,12 @@
         <v>27</v>
       </c>
       <c r="B31" s="5">
-        <f>713040</f>
-        <v>713040</v>
+        <f>4023287</f>
+        <v>4023287</v>
       </c>
       <c r="C31" s="5">
-        <f>743123</f>
-        <v>743123</v>
+        <f>3890931</f>
+        <v>3890931</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1236,12 +1251,12 @@
         <v>28</v>
       </c>
       <c r="B32" s="5">
-        <f>1495600</f>
-        <v>1495600</v>
+        <f>5914882</f>
+        <v>5914882</v>
       </c>
       <c r="C32" s="5">
-        <f>1476929</f>
-        <v>1476929</v>
+        <f>5769558</f>
+        <v>5769558</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1249,12 +1264,12 @@
         <v>29</v>
       </c>
       <c r="B33" s="5">
-        <f>184600</f>
-        <v>184600</v>
+        <f>1402006</f>
+        <v>1402006</v>
       </c>
       <c r="C33" s="5">
-        <f>182071</f>
-        <v>182071</v>
+        <f>882653</f>
+        <v>882653</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1262,12 +1277,12 @@
         <v>30</v>
       </c>
       <c r="B34" s="5">
-        <f>2465376</f>
-        <v>2465376</v>
+        <f>15561741</f>
+        <v>15561741</v>
       </c>
       <c r="C34" s="5">
-        <f>3956769</f>
-        <v>3956769</v>
+        <f>14325630.78</f>
+        <v>14325630.779999999</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1276,11 +1291,11 @@
       </c>
       <c r="B35" s="6">
         <f>(((((B29)+(B30))+(B31))+(B32))+(B33))+(B34)</f>
-        <v>5970940</v>
+        <v>34278172</v>
       </c>
       <c r="C35" s="6">
         <f>(((((C29)+(C30))+(C31))+(C32))+(C33))+(C34)</f>
-        <v>7201570</v>
+        <v>33561945.539999999</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1288,12 +1303,12 @@
         <v>32</v>
       </c>
       <c r="B36" s="5">
-        <f>1003234</f>
-        <v>1003234</v>
+        <f>6995449</f>
+        <v>6995449</v>
       </c>
       <c r="C36" s="5">
-        <f>3315362</f>
-        <v>3315362</v>
+        <f>9884767</f>
+        <v>9884767</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1301,12 +1316,12 @@
         <v>33</v>
       </c>
       <c r="B37" s="5">
-        <f>2026929</f>
-        <v>2026929</v>
+        <f>15304457</f>
+        <v>15304457</v>
       </c>
       <c r="C37" s="5">
-        <f>2363424</f>
-        <v>2363424</v>
+        <f>12683930.74</f>
+        <v>12683930.74</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,12 +1329,12 @@
         <v>34</v>
       </c>
       <c r="B38" s="5">
-        <f>1246260</f>
-        <v>1246260</v>
+        <f>8669529</f>
+        <v>8669529</v>
       </c>
       <c r="C38" s="5">
-        <f>1650764</f>
-        <v>1650764</v>
+        <f>8412028</f>
+        <v>8412028</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1327,12 +1342,12 @@
         <v>35</v>
       </c>
       <c r="B39" s="5">
-        <f>1247896</f>
-        <v>1247896</v>
+        <f>5594702</f>
+        <v>5594702</v>
       </c>
       <c r="C39" s="5">
-        <f>1085842</f>
-        <v>1085842</v>
+        <f>4556449.65</f>
+        <v>4556449.6500000004</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1340,12 +1355,12 @@
         <v>36</v>
       </c>
       <c r="B40" s="5">
-        <f>984735</f>
-        <v>984735</v>
+        <f>6536746.6</f>
+        <v>6536746.5999999996</v>
       </c>
       <c r="C40" s="5">
-        <f>655929</f>
-        <v>655929</v>
+        <f>7117116</f>
+        <v>7117116</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1353,12 +1368,12 @@
         <v>37</v>
       </c>
       <c r="B41" s="5">
-        <f>1897035</f>
-        <v>1897035</v>
+        <f>5742937</f>
+        <v>5742937</v>
       </c>
       <c r="C41" s="5">
-        <f>2561049</f>
-        <v>2561049</v>
+        <f>7373230</f>
+        <v>7373230</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1367,11 +1382,11 @@
       </c>
       <c r="B42" s="6">
         <f>((((((((B22)+(B28))+(B35))+(B36))+(B37))+(B38))+(B39))+(B40))+(B41)</f>
-        <v>21491971</v>
+        <v>148349313.59999999</v>
       </c>
       <c r="C42" s="6">
         <f>((((((((C22)+(C28))+(C35))+(C36))+(C37))+(C38))+(C39))+(C40))+(C41)</f>
-        <v>35551588</v>
+        <v>152548588.20999998</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1386,12 +1401,12 @@
         <v>40</v>
       </c>
       <c r="B44" s="5">
-        <f>4811031</f>
-        <v>4811031</v>
+        <f>41346905</f>
+        <v>41346905</v>
       </c>
       <c r="C44" s="5">
-        <f>4896145</f>
-        <v>4896145</v>
+        <f>35983987.33</f>
+        <v>35983987.329999998</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1399,12 +1414,12 @@
         <v>41</v>
       </c>
       <c r="B45" s="5">
-        <f>871410</f>
-        <v>871410</v>
+        <f>6910950</f>
+        <v>6910950</v>
       </c>
       <c r="C45" s="5">
-        <f>2048680</f>
-        <v>2048680</v>
+        <f>5625265</f>
+        <v>5625265</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1412,12 +1427,12 @@
         <v>42</v>
       </c>
       <c r="B46" s="5">
-        <f>868432</f>
-        <v>868432</v>
+        <f>7100965</f>
+        <v>7100965</v>
       </c>
       <c r="C46" s="5">
-        <f>1241898</f>
-        <v>1241898</v>
+        <f>8354416</f>
+        <v>8354416</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1426,11 +1441,11 @@
       </c>
       <c r="B47" s="6">
         <f>(((B43)+(B44))+(B45))+(B46)</f>
-        <v>6550873</v>
+        <v>55358820</v>
       </c>
       <c r="C47" s="6">
         <f>(((C43)+(C44))+(C45))+(C46)</f>
-        <v>8186723</v>
+        <v>49963668.329999998</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1445,12 +1460,12 @@
         <v>45</v>
       </c>
       <c r="B49" s="5">
-        <f>1500328</f>
-        <v>1500328</v>
+        <f>13197737</f>
+        <v>13197737</v>
       </c>
       <c r="C49" s="5">
-        <f>1206500</f>
-        <v>1206500</v>
+        <f>10508556</f>
+        <v>10508556</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1458,12 +1473,12 @@
         <v>46</v>
       </c>
       <c r="B50" s="5">
-        <f>2849518</f>
-        <v>2849518</v>
+        <f>17422851.79</f>
+        <v>17422851.789999999</v>
       </c>
       <c r="C50" s="5">
-        <f>2556204</f>
-        <v>2556204</v>
+        <f>12200143</f>
+        <v>12200143</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1471,12 +1486,12 @@
         <v>47</v>
       </c>
       <c r="B51" s="5">
-        <f>1384180</f>
-        <v>1384180</v>
+        <f>12291882</f>
+        <v>12291882</v>
       </c>
       <c r="C51" s="5">
-        <f>2052728</f>
-        <v>2052728</v>
+        <f>13212231.3</f>
+        <v>13212231.300000001</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1484,12 +1499,12 @@
         <v>48</v>
       </c>
       <c r="B52" s="5">
-        <f>121150</f>
-        <v>121150</v>
+        <f>1805990</f>
+        <v>1805990</v>
       </c>
       <c r="C52" s="5">
-        <f>680725</f>
-        <v>680725</v>
+        <f>2415726</f>
+        <v>2415726</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1497,12 +1512,12 @@
         <v>49</v>
       </c>
       <c r="B53" s="5">
-        <f>184821</f>
-        <v>184821</v>
+        <f>1001124</f>
+        <v>1001124</v>
       </c>
       <c r="C53" s="5">
-        <f>175923</f>
-        <v>175923</v>
+        <f>1237494</f>
+        <v>1237494</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1510,12 +1525,12 @@
         <v>50</v>
       </c>
       <c r="B54" s="5">
-        <f>14625</f>
-        <v>14625</v>
+        <f>2181098</f>
+        <v>2181098</v>
       </c>
       <c r="C54" s="5">
-        <f>2098970</f>
-        <v>2098970</v>
+        <f>3069841</f>
+        <v>3069841</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,22 +1538,25 @@
         <v>51</v>
       </c>
       <c r="B55" s="5">
-        <f>225246</f>
-        <v>225246</v>
+        <f>2114206</f>
+        <v>2114206</v>
       </c>
       <c r="C55" s="5">
-        <f>142569</f>
-        <v>142569</v>
+        <f>1604134</f>
+        <v>1604134</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="4"/>
+      <c r="B56" s="5">
+        <f>883200</f>
+        <v>883200</v>
+      </c>
       <c r="C56" s="5">
-        <f>295000</f>
-        <v>295000</v>
+        <f>425000</f>
+        <v>425000</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1547,11 +1565,11 @@
       </c>
       <c r="B57" s="6">
         <f>((((((((B48)+(B49))+(B50))+(B51))+(B52))+(B53))+(B54))+(B55))+(B56)</f>
-        <v>6279868</v>
+        <v>50898088.789999999</v>
       </c>
       <c r="C57" s="6">
         <f>((((((((C48)+(C49))+(C50))+(C51))+(C52))+(C53))+(C54))+(C55))+(C56)</f>
-        <v>9208619</v>
+        <v>44673125.299999997</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,11 +1578,11 @@
       </c>
       <c r="B58" s="6">
         <f>((B42)+(B47))+(B57)</f>
-        <v>34322712</v>
+        <v>254606222.38999999</v>
       </c>
       <c r="C58" s="6">
         <f>((C42)+(C47))+(C57)</f>
-        <v>52946930</v>
+        <v>247185381.83999997</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -1573,11 +1591,11 @@
       </c>
       <c r="B59" s="6">
         <f>(B20)-(B58)</f>
-        <v>10806021.5</v>
+        <v>78171178.300000012</v>
       </c>
       <c r="C59" s="6">
         <f>(C20)-(C58)</f>
-        <v>21457044.459999993</v>
+        <v>84580375.600000083</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1599,12 +1617,12 @@
         <v>58</v>
       </c>
       <c r="B62" s="5">
-        <f>6806986</f>
-        <v>6806986</v>
+        <f>55434336</f>
+        <v>55434336</v>
       </c>
       <c r="C62" s="5">
-        <f>1684200</f>
-        <v>1684200</v>
+        <f>36022691</f>
+        <v>36022691</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1612,12 +1630,12 @@
         <v>59</v>
       </c>
       <c r="B63" s="5">
-        <f>843803</f>
-        <v>843803</v>
+        <f>8682243.5</f>
+        <v>8682243.5</v>
       </c>
       <c r="C63" s="5">
-        <f>937247</f>
-        <v>937247</v>
+        <f>5866710.52</f>
+        <v>5866710.5199999996</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1626,11 +1644,11 @@
       </c>
       <c r="B64" s="6">
         <f>((B61)+(B62))+(B63)</f>
-        <v>7650789</v>
+        <v>64116579.5</v>
       </c>
       <c r="C64" s="6">
         <f>((C61)+(C62))+(C63)</f>
-        <v>2621447</v>
+        <v>41889401.519999996</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1639,11 +1657,11 @@
       </c>
       <c r="B65" s="6">
         <f>B64</f>
-        <v>7650789</v>
+        <v>64116579.5</v>
       </c>
       <c r="C65" s="6">
         <f>C64</f>
-        <v>2621447</v>
+        <v>41889401.519999996</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -1665,19 +1683,22 @@
         <v>64</v>
       </c>
       <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
+      <c r="C68" s="5">
+        <f>8357523.67</f>
+        <v>8357523.6699999999</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B69" s="5">
-        <f>629600</f>
-        <v>629600</v>
+        <f>5879250</f>
+        <v>5879250</v>
       </c>
       <c r="C69" s="5">
-        <f>644900</f>
-        <v>644900</v>
+        <f>2019583</f>
+        <v>2019583</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1685,12 +1706,12 @@
         <v>66</v>
       </c>
       <c r="B70" s="5">
-        <f>0</f>
-        <v>0</v>
+        <f>403667</f>
+        <v>403667</v>
       </c>
       <c r="C70" s="5">
-        <f>174200</f>
-        <v>174200</v>
+        <f>783333</f>
+        <v>783333</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1698,12 +1719,12 @@
         <v>67</v>
       </c>
       <c r="B71" s="5">
-        <f>1179148</f>
-        <v>1179148</v>
+        <f>9639449</f>
+        <v>9639449</v>
       </c>
       <c r="C71" s="5">
-        <f>852431</f>
-        <v>852431</v>
+        <f>2308648</f>
+        <v>2308648</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1711,12 +1732,12 @@
         <v>68</v>
       </c>
       <c r="B72" s="5">
-        <f>495000</f>
-        <v>495000</v>
+        <f>3327771</f>
+        <v>3327771</v>
       </c>
       <c r="C72" s="5">
-        <f>271679</f>
-        <v>271679</v>
+        <f>934851</f>
+        <v>934851</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1725,11 +1746,11 @@
       </c>
       <c r="B73" s="6">
         <f>((((B68)+(B69))+(B70))+(B71))+(B72)</f>
-        <v>2303748</v>
+        <v>19250137</v>
       </c>
       <c r="C73" s="6">
         <f>((((C68)+(C69))+(C70))+(C71))+(C72)</f>
-        <v>1943210</v>
+        <v>14403938.67</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1737,12 +1758,12 @@
         <v>70</v>
       </c>
       <c r="B74" s="5">
-        <f>273649.25</f>
-        <v>273649.25</v>
+        <f>2445084.25</f>
+        <v>2445084.25</v>
       </c>
       <c r="C74" s="5">
-        <f>207332.25</f>
-        <v>207332.25</v>
+        <f>1480077.75</f>
+        <v>1480077.75</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -1756,10 +1777,13 @@
       <c r="A76" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="4"/>
+      <c r="B76" s="5">
+        <f>3022807</f>
+        <v>3022807</v>
+      </c>
       <c r="C76" s="5">
-        <f>792836</f>
-        <v>792836</v>
+        <f>2321785</f>
+        <v>2321785</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -1768,8 +1792,8 @@
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="5">
-        <f>153570.81</f>
-        <v>153570.81</v>
+        <f>3037878.37</f>
+        <v>3037878.37</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -1778,11 +1802,11 @@
       </c>
       <c r="B78" s="6">
         <f>((B75)+(B76))+(B77)</f>
-        <v>0</v>
+        <v>3022807</v>
       </c>
       <c r="C78" s="6">
         <f>((C75)+(C76))+(C77)</f>
-        <v>946406.81</v>
+        <v>5359663.37</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -1791,11 +1815,11 @@
       </c>
       <c r="B79" s="6">
         <f>(((B67)+(B73))+(B74))+(B78)</f>
-        <v>2577397.25</v>
+        <v>24718028.25</v>
       </c>
       <c r="C79" s="6">
         <f>(((C67)+(C73))+(C74))+(C78)</f>
-        <v>3096949.06</v>
+        <v>21243679.789999999</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1810,114 +1834,111 @@
         <v>77</v>
       </c>
       <c r="B81" s="5">
-        <f>323800</f>
-        <v>323800</v>
+        <f>2800700</f>
+        <v>2800700</v>
       </c>
       <c r="C81" s="5">
-        <f>232500</f>
-        <v>232500</v>
+        <f>1697583</f>
+        <v>1697583</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="5">
-        <f>2680</f>
-        <v>2680</v>
-      </c>
+      <c r="B82" s="4"/>
       <c r="C82" s="5">
-        <f>340</f>
-        <v>340</v>
+        <f>27500</f>
+        <v>27500</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B83" s="6">
-        <f>((B80)+(B81))+(B82)</f>
-        <v>326480</v>
-      </c>
-      <c r="C83" s="6">
-        <f>((C80)+(C81))+(C82)</f>
-        <v>232840</v>
+      <c r="B83" s="5">
+        <f>6790</f>
+        <v>6790</v>
+      </c>
+      <c r="C83" s="5">
+        <f>6970</f>
+        <v>6970</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
+      <c r="B84" s="6">
+        <f>(((B80)+(B81))+(B82))+(B83)</f>
+        <v>2807490</v>
+      </c>
+      <c r="C84" s="6">
+        <f>(((C80)+(C81))+(C82))+(C83)</f>
+        <v>1732053</v>
+      </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B85" s="5">
-        <f>165566</f>
-        <v>165566</v>
-      </c>
-      <c r="C85" s="5">
-        <f>79009</f>
-        <v>79009</v>
-      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B86" s="5">
-        <f>2000</f>
-        <v>2000</v>
+        <f>1598528</f>
+        <v>1598528</v>
       </c>
       <c r="C86" s="5">
-        <f>4320</f>
-        <v>4320</v>
+        <f>756247</f>
+        <v>756247</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B87" s="6">
-        <f>((B84)+(B85))+(B86)</f>
-        <v>167566</v>
-      </c>
-      <c r="C87" s="6">
-        <f>((C84)+(C85))+(C86)</f>
-        <v>83329</v>
-      </c>
+      <c r="B87" s="5">
+        <f>129290</f>
+        <v>129290</v>
+      </c>
+      <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
+      <c r="B88" s="5">
+        <f>50020</f>
+        <v>50020</v>
+      </c>
+      <c r="C88" s="5">
+        <f>70740</f>
+        <v>70740</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="5">
-        <f>32000</f>
-        <v>32000</v>
-      </c>
-      <c r="C89" s="5">
-        <f>32000</f>
-        <v>32000</v>
+      <c r="B89" s="6">
+        <f>(((B85)+(B86))+(B87))+(B88)</f>
+        <v>1777838</v>
+      </c>
+      <c r="C89" s="6">
+        <f>(((C85)+(C86))+(C87))+(C88)</f>
+        <v>826987</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B90" s="5">
-        <f>120000</f>
-        <v>120000</v>
-      </c>
+      <c r="B90" s="4"/>
       <c r="C90" s="4"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -1925,196 +1946,199 @@
         <v>87</v>
       </c>
       <c r="B91" s="5">
-        <f>591600</f>
-        <v>591600</v>
-      </c>
-      <c r="C91" s="5">
-        <f>496250</f>
-        <v>496250</v>
-      </c>
+        <f>32000</f>
+        <v>32000</v>
+      </c>
+      <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B92" s="5">
-        <f>191629</f>
-        <v>191629</v>
+        <f>288000</f>
+        <v>288000</v>
       </c>
       <c r="C92" s="5">
-        <f>2084329.06</f>
-        <v>2084329.06</v>
+        <f>288000</f>
+        <v>288000</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B93" s="6">
-        <f>((((B88)+(B89))+(B90))+(B91))+(B92)</f>
-        <v>935229</v>
-      </c>
-      <c r="C93" s="6">
-        <f>((((C88)+(C89))+(C90))+(C91))+(C92)</f>
-        <v>2612579.06</v>
-      </c>
+      <c r="B93" s="5">
+        <f>120000</f>
+        <v>120000</v>
+      </c>
+      <c r="C93" s="4"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
+      <c r="B94" s="5">
+        <f>4789650</f>
+        <v>4789650</v>
+      </c>
+      <c r="C94" s="5">
+        <f>4308401.5</f>
+        <v>4308401.5</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B95" s="5">
-        <f>24905</f>
-        <v>24905</v>
-      </c>
-      <c r="C95" s="5">
-        <f>19609</f>
-        <v>19609</v>
-      </c>
+        <f>30770</f>
+        <v>30770</v>
+      </c>
+      <c r="C95" s="4"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B96" s="5">
-        <f>104173</f>
-        <v>104173</v>
+        <f>3280680.47</f>
+        <v>3280680.47</v>
       </c>
       <c r="C96" s="5">
-        <f>72378</f>
-        <v>72378</v>
+        <f>2846447.9</f>
+        <v>2846447.9</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B97" s="5">
-        <f>1760</f>
-        <v>1760</v>
-      </c>
-      <c r="C97" s="5">
-        <f>10000</f>
-        <v>10000</v>
+      <c r="B97" s="6">
+        <f>((((((B90)+(B91))+(B92))+(B93))+(B94))+(B95))+(B96)</f>
+        <v>8541100.4700000007</v>
+      </c>
+      <c r="C97" s="6">
+        <f>((((((C90)+(C91))+(C92))+(C93))+(C94))+(C95))+(C96)</f>
+        <v>7442849.4000000004</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B98" s="5">
-        <f>6420</f>
-        <v>6420</v>
-      </c>
-      <c r="C98" s="5">
-        <f>4670</f>
-        <v>4670</v>
-      </c>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B99" s="6">
-        <f>((((B94)+(B95))+(B96))+(B97))+(B98)</f>
-        <v>137258</v>
-      </c>
-      <c r="C99" s="6">
-        <f>((((C94)+(C95))+(C96))+(C97))+(C98)</f>
-        <v>106657</v>
+      <c r="B99" s="5">
+        <f>220383</f>
+        <v>220383</v>
+      </c>
+      <c r="C99" s="5">
+        <f>193694</f>
+        <v>193694</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
+      <c r="B100" s="5">
+        <f>747479.21</f>
+        <v>747479.21</v>
+      </c>
+      <c r="C100" s="5">
+        <f>465364</f>
+        <v>465364</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B101" s="5">
-        <f>5600</f>
-        <v>5600</v>
-      </c>
-      <c r="C101" s="4"/>
+        <f>12849</f>
+        <v>12849</v>
+      </c>
+      <c r="C101" s="5">
+        <f>31456</f>
+        <v>31456</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B102" s="5">
-        <f>4700</f>
-        <v>4700</v>
+        <f>48920</f>
+        <v>48920</v>
       </c>
       <c r="C102" s="5">
-        <f>30000</f>
-        <v>30000</v>
+        <f>36939</f>
+        <v>36939</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B103" s="5">
-        <f>12819</f>
-        <v>12819</v>
-      </c>
-      <c r="C103" s="5">
-        <f>11397</f>
-        <v>11397</v>
+      <c r="B103" s="6">
+        <f>((((B98)+(B99))+(B100))+(B101))+(B102)</f>
+        <v>1029631.21</v>
+      </c>
+      <c r="C103" s="6">
+        <f>((((C98)+(C99))+(C100))+(C101))+(C102)</f>
+        <v>727453</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B104" s="6">
-        <f>(((B100)+(B101))+(B102))+(B103)</f>
-        <v>23119</v>
-      </c>
-      <c r="C104" s="6">
-        <f>(((C100)+(C101))+(C102))+(C103)</f>
-        <v>41397</v>
-      </c>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
+      <c r="B105" s="5">
+        <f>257905</f>
+        <v>257905</v>
+      </c>
+      <c r="C105" s="5">
+        <f>41900</f>
+        <v>41900</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B106" s="5">
-        <f>177584</f>
-        <v>177584</v>
+        <f>275954</f>
+        <v>275954</v>
       </c>
       <c r="C106" s="5">
-        <f>422620</f>
-        <v>422620</v>
+        <f>204125</f>
+        <v>204125</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B107" s="4"/>
+      <c r="B107" s="5">
+        <f>492164</f>
+        <v>492164</v>
+      </c>
       <c r="C107" s="5">
-        <f>0</f>
-        <v>0</v>
+        <f>225887</f>
+        <v>225887</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2122,12 +2146,12 @@
         <v>104</v>
       </c>
       <c r="B108" s="6">
-        <f>((B105)+(B106))+(B107)</f>
-        <v>177584</v>
+        <f>(((B104)+(B105))+(B106))+(B107)</f>
+        <v>1026023</v>
       </c>
       <c r="C108" s="6">
-        <f>((C105)+(C106))+(C107)</f>
-        <v>422620</v>
+        <f>(((C104)+(C105))+(C106))+(C107)</f>
+        <v>471912</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2142,12 +2166,12 @@
         <v>106</v>
       </c>
       <c r="B110" s="5">
-        <f>91198</f>
-        <v>91198</v>
+        <f>3789629</f>
+        <v>3789629</v>
       </c>
       <c r="C110" s="5">
-        <f>33542</f>
-        <v>33542</v>
+        <f>3003078</f>
+        <v>3003078</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2155,12 +2179,12 @@
         <v>107</v>
       </c>
       <c r="B111" s="5">
-        <f>2580</f>
-        <v>2580</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="C111" s="5">
-        <f>58170</f>
-        <v>58170</v>
+        <f>32530</f>
+        <v>32530</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2169,11 +2193,11 @@
       </c>
       <c r="B112" s="6">
         <f>((B109)+(B110))+(B111)</f>
-        <v>93778</v>
+        <v>3789629</v>
       </c>
       <c r="C112" s="6">
         <f>((C109)+(C110))+(C111)</f>
-        <v>91712</v>
+        <v>3035608</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2188,12 +2212,12 @@
         <v>110</v>
       </c>
       <c r="B114" s="5">
-        <f>140000</f>
-        <v>140000</v>
+        <f>463537</f>
+        <v>463537</v>
       </c>
       <c r="C114" s="5">
-        <f>0</f>
-        <v>0</v>
+        <f>227642</f>
+        <v>227642</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2201,55 +2225,58 @@
         <v>111</v>
       </c>
       <c r="B115" s="5">
-        <f>120576</f>
-        <v>120576</v>
+        <f>352883</f>
+        <v>352883</v>
       </c>
       <c r="C115" s="5">
-        <f>224556.99</f>
-        <v>224556.99</v>
+        <f>377189</f>
+        <v>377189</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="5">
-        <f>130000</f>
-        <v>130000</v>
+      <c r="B116" s="6">
+        <f>((B113)+(B114))+(B115)</f>
+        <v>816420</v>
+      </c>
+      <c r="C116" s="6">
+        <f>((C113)+(C114))+(C115)</f>
+        <v>604831</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B117" s="6">
-        <f>(((B113)+(B114))+(B115))+(B116)</f>
-        <v>260576</v>
-      </c>
-      <c r="C117" s="6">
-        <f>(((C113)+(C114))+(C115))+(C116)</f>
-        <v>354556.99</v>
-      </c>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
+      <c r="B118" s="5">
+        <f>1380000</f>
+        <v>1380000</v>
+      </c>
+      <c r="C118" s="5">
+        <f>783750</f>
+        <v>783750</v>
+      </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B119" s="5">
-        <f>38658</f>
-        <v>38658</v>
+        <f>2509617.52</f>
+        <v>2509617.52</v>
       </c>
       <c r="C119" s="5">
-        <f>14835</f>
-        <v>14835</v>
+        <f>1514299.81</f>
+        <v>1514299.81</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2257,12 +2284,12 @@
         <v>116</v>
       </c>
       <c r="B120" s="5">
-        <f>13970</f>
-        <v>13970</v>
+        <f>40000</f>
+        <v>40000</v>
       </c>
       <c r="C120" s="5">
-        <f>26909</f>
-        <v>26909</v>
+        <f>229446</f>
+        <v>229446</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2270,148 +2297,194 @@
         <v>117</v>
       </c>
       <c r="B121" s="6">
-        <f>((B118)+(B119))+(B120)</f>
-        <v>52628</v>
+        <f>(((B117)+(B118))+(B119))+(B120)</f>
+        <v>3929617.52</v>
       </c>
       <c r="C121" s="6">
-        <f>((C118)+(C119))+(C120)</f>
-        <v>41744</v>
+        <f>(((C117)+(C118))+(C119))+(C120)</f>
+        <v>2527495.81</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B122" s="6">
-        <f>(((((((((B79)+(B83))+(B87))+(B93))+(B99))+(B104))+(B108))+(B112))+(B117))+(B121)</f>
-        <v>4751615.25</v>
-      </c>
-      <c r="C122" s="6">
-        <f>(((((((((C79)+(C83))+(C87))+(C93))+(C99))+(C104))+(C108))+(C112))+(C117))+(C121)</f>
-        <v>7084384.1100000003</v>
-      </c>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
+      <c r="B123" s="5">
+        <f>143870.39</f>
+        <v>143870.39000000001</v>
+      </c>
+      <c r="C123" s="5">
+        <f>155572</f>
+        <v>155572</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
+      <c r="B124" s="5">
+        <f>209201</f>
+        <v>209201</v>
+      </c>
+      <c r="C124" s="5">
+        <f>219981</f>
+        <v>219981</v>
+      </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B125" s="5">
-        <f>2045660</f>
-        <v>2045660</v>
-      </c>
-      <c r="C125" s="5">
-        <f>1981350</f>
-        <v>1981350</v>
+      <c r="B125" s="6">
+        <f>((B122)+(B123))+(B124)</f>
+        <v>353071.39</v>
+      </c>
+      <c r="C125" s="6">
+        <f>((C122)+(C123))+(C124)</f>
+        <v>375553</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B126" s="5">
-        <f>25625.6</f>
-        <v>25625.599999999999</v>
-      </c>
-      <c r="C126" s="5">
-        <f>32507.17</f>
-        <v>32507.17</v>
+      <c r="B126" s="6">
+        <f>(((((((((B79)+(B84))+(B89))+(B97))+(B103))+(B108))+(B112))+(B116))+(B121))+(B125)</f>
+        <v>48788848.840000004</v>
+      </c>
+      <c r="C126" s="6">
+        <f>(((((((((C79)+(C84))+(C89))+(C97))+(C103))+(C108))+(C112))+(C116))+(C121))+(C125)</f>
+        <v>38988422</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B127" s="5">
-        <f>44906</f>
-        <v>44906</v>
-      </c>
-      <c r="C127" s="5">
-        <f>251537.64</f>
-        <v>251537.64</v>
-      </c>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B128" s="5">
-        <f>1193454</f>
-        <v>1193454</v>
-      </c>
-      <c r="C128" s="5">
-        <f>1945110</f>
-        <v>1945110</v>
-      </c>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B129" s="6">
-        <f>((((B124)+(B125))+(B126))+(B127))+(B128)</f>
-        <v>3309645.6</v>
-      </c>
-      <c r="C129" s="6">
-        <f>((((C124)+(C125))+(C126))+(C127))+(C128)</f>
-        <v>4210504.8100000005</v>
+      <c r="B129" s="5">
+        <f>26320006</f>
+        <v>26320006</v>
+      </c>
+      <c r="C129" s="5">
+        <f>30439970</f>
+        <v>30439970</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B130" s="6">
-        <f>B129</f>
-        <v>3309645.6</v>
-      </c>
-      <c r="C130" s="6">
-        <f>C129</f>
-        <v>4210504.8100000005</v>
+      <c r="B130" s="5">
+        <f>284725.23</f>
+        <v>284725.23</v>
+      </c>
+      <c r="C130" s="5">
+        <f>100473.75</f>
+        <v>100473.75</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B131" s="7">
-        <f>((((B20)+(B65))-(B58))-(B122))-(B130)</f>
-        <v>10395549.65</v>
-      </c>
-      <c r="C131" s="7">
-        <f>((((C20)+(C65))-(C58))-(C122))-(C130)</f>
-        <v>12783602.539999994</v>
+      <c r="B131" s="5">
+        <f>153555</f>
+        <v>153555</v>
+      </c>
+      <c r="C131" s="5">
+        <f>4949160.1</f>
+        <v>4949160.0999999996</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="3"/>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
+      <c r="A132" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B132" s="5">
+        <f>12796500</f>
+        <v>12796500</v>
+      </c>
+      <c r="C132" s="5">
+        <f>10029516</f>
+        <v>10029516</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B133" s="6">
+        <f>((((B128)+(B129))+(B130))+(B131))+(B132)</f>
+        <v>39554786.230000004</v>
+      </c>
+      <c r="C133" s="6">
+        <f>((((C128)+(C129))+(C130))+(C131))+(C132)</f>
+        <v>45519119.850000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B134" s="6">
+        <f>B133</f>
+        <v>39554786.230000004</v>
+      </c>
+      <c r="C134" s="6">
+        <f>C133</f>
+        <v>45519119.850000001</v>
+      </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B135" s="11"/>
-      <c r="C135" s="11"/>
+      <c r="A135" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B135" s="7">
+        <f>((((B20)+(B65))-(B58))-(B126))-(B134)</f>
+        <v>53944122.730000004</v>
+      </c>
+      <c r="C135" s="7">
+        <f>((((C20)+(C65))-(C58))-(C126))-(C134)</f>
+        <v>41962235.270000063</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="3"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B139" s="11"/>
+      <c r="C139" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>

</xml_diff>